<commit_message>
Ticket 9519 corrected calibration sheet with input from Steve Gaul and Sheri White.
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CP03ISSM_00002.xlsx
+++ b/deployment/Omaha_Cal_Info_CP03ISSM_00002.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauls\Desktop\Temp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="735" yWindow="405" windowWidth="20730" windowHeight="7020" tabRatio="766" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14220" windowHeight="8436" tabRatio="766" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
     <sheet name="ACS130_CC_taarray" sheetId="5" r:id="rId5"/>
     <sheet name="ACS130_CC_tcarray" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="236">
   <si>
     <t>Ref Des</t>
   </si>
@@ -671,13 +676,7 @@
     <t>CP03ISSM-00002-METBK</t>
   </si>
   <si>
-    <t>CP03ISSM-00002-SBD11-02-HYDGN0000</t>
-  </si>
-  <si>
     <t>CP03ISSM-00002-MOPAK</t>
-  </si>
-  <si>
-    <t>CP03ISSM-00002-SBD12-03-HYDGN0000</t>
   </si>
   <si>
     <t>CP03ISSM-00002-CPM1</t>
@@ -709,6 +708,48 @@
   <si>
     <t>N00756</t>
   </si>
+  <si>
+    <t>R00012</t>
+  </si>
+  <si>
+    <t>R00013</t>
+  </si>
+  <si>
+    <t>R00014</t>
+  </si>
+  <si>
+    <t>R00015</t>
+  </si>
+  <si>
+    <t>R00016</t>
+  </si>
+  <si>
+    <t>R00017</t>
+  </si>
+  <si>
+    <t>R00018</t>
+  </si>
+  <si>
+    <t>R00019</t>
+  </si>
+  <si>
+    <t>R00020</t>
+  </si>
+  <si>
+    <t>R00021</t>
+  </si>
+  <si>
+    <t>R00022</t>
+  </si>
+  <si>
+    <t>R00023</t>
+  </si>
+  <si>
+    <t>CP03ISSM-00002-HYDGN1</t>
+  </si>
+  <si>
+    <t>CP03ISSM-00002-HYDGN2</t>
+  </si>
 </sst>
 </file>
 
@@ -718,7 +759,7 @@
     <numFmt numFmtId="164" formatCode="d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -786,8 +827,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -824,8 +872,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -884,6 +938,21 @@
       </top>
       <bottom style="hair">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -971,7 +1040,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1079,6 +1148,9 @@
     </xf>
     <xf numFmtId="165" fontId="8" fillId="6" borderId="4" xfId="80" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="81">
@@ -1573,23 +1645,23 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="1"/>
-    <col min="3" max="3" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="3"/>
-    <col min="7" max="7" width="8.85546875" style="2"/>
-    <col min="8" max="8" width="14.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" style="1" customWidth="1"/>
-    <col min="10" max="11" width="8.85546875" style="1"/>
-    <col min="12" max="12" width="35.42578125" style="1" customWidth="1"/>
-    <col min="13" max="1026" width="8.85546875" style="1"/>
+    <col min="6" max="6" width="8.88671875" style="3"/>
+    <col min="7" max="7" width="8.88671875" style="2"/>
+    <col min="8" max="8" width="14.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" style="1" customWidth="1"/>
+    <col min="10" max="11" width="8.88671875" style="1"/>
+    <col min="12" max="12" width="35.44140625" style="1" customWidth="1"/>
+    <col min="13" max="1026" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1026" s="9" customFormat="1" ht="38.25">
+    <row r="1" spans="1:1026" s="9" customFormat="1" ht="41.4">
       <c r="A1" s="37" t="s">
         <v>183</v>
       </c>
@@ -2694,25 +2766,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMM194"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7:E15"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="27.140625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.42578125" style="14" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="39.7109375" style="14" customWidth="1"/>
-    <col min="8" max="8" width="46.28515625" style="14" customWidth="1"/>
-    <col min="9" max="9" width="55.7109375" style="14" customWidth="1"/>
-    <col min="10" max="1027" width="8.85546875" style="14"/>
+    <col min="1" max="2" width="27.109375" style="14" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.44140625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.6640625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="46.33203125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="55.6640625" style="14" customWidth="1"/>
+    <col min="10" max="1027" width="8.88671875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1026" s="16" customFormat="1" ht="12.75">
+    <row r="1" spans="1:1026" s="16" customFormat="1" ht="13.8">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -3782,8 +3854,11 @@
       <c r="D3" s="14">
         <v>2</v>
       </c>
+      <c r="E3" s="40" t="s">
+        <v>222</v>
+      </c>
       <c r="F3" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G3"/>
       <c r="H3"/>
@@ -4821,8 +4896,11 @@
       <c r="D5" s="26">
         <v>2</v>
       </c>
-      <c r="F5" s="18" t="s">
-        <v>211</v>
+      <c r="E5" s="40" t="s">
+        <v>223</v>
+      </c>
+      <c r="F5" s="40" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:1026">
@@ -4839,7 +4917,7 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F7" t="s">
         <v>210</v>
@@ -5885,7 +5963,7 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F8" t="s">
         <v>210</v>
@@ -6931,7 +7009,7 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F9" t="s">
         <v>210</v>
@@ -7977,7 +8055,7 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F10" t="s">
         <v>210</v>
@@ -9023,7 +9101,7 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F11" t="s">
         <v>210</v>
@@ -10069,7 +10147,7 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F12" t="s">
         <v>210</v>
@@ -11115,7 +11193,7 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F13" t="s">
         <v>210</v>
@@ -12161,7 +12239,7 @@
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F14" t="s">
         <v>210</v>
@@ -13207,7 +13285,7 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F15" t="s">
         <v>210</v>
@@ -15280,8 +15358,11 @@
       <c r="D17" s="26">
         <v>2</v>
       </c>
-      <c r="F17" s="18" t="s">
-        <v>213</v>
+      <c r="E17" s="40" t="s">
+        <v>224</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="19" spans="1:1026">
@@ -51893,8 +51974,11 @@
       <c r="D180" s="14">
         <v>2</v>
       </c>
+      <c r="E180" s="40" t="s">
+        <v>225</v>
+      </c>
       <c r="F180" s="18" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I180" s="29" t="s">
         <v>132</v>
@@ -51914,8 +51998,11 @@
       <c r="D181" s="14">
         <v>2</v>
       </c>
+      <c r="E181" s="40" t="s">
+        <v>226</v>
+      </c>
       <c r="F181" s="18" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I181" s="29" t="s">
         <v>132</v>
@@ -51935,8 +52022,11 @@
       <c r="D182" s="14">
         <v>2</v>
       </c>
+      <c r="E182" s="40" t="s">
+        <v>227</v>
+      </c>
       <c r="F182" s="18" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I182" s="29" t="s">
         <v>132</v>
@@ -51966,8 +52056,11 @@
       <c r="D184" s="14">
         <v>2</v>
       </c>
+      <c r="E184" s="40" t="s">
+        <v>228</v>
+      </c>
       <c r="F184" s="18" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I184" s="29" t="s">
         <v>136</v>
@@ -51987,8 +52080,11 @@
       <c r="D185" s="14">
         <v>2</v>
       </c>
+      <c r="E185" s="40" t="s">
+        <v>229</v>
+      </c>
       <c r="F185" s="18" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I185" s="29" t="s">
         <v>136</v>
@@ -52008,8 +52104,11 @@
       <c r="D186" s="14">
         <v>2</v>
       </c>
+      <c r="E186" s="40" t="s">
+        <v>230</v>
+      </c>
       <c r="F186" s="18" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="I186" s="29" t="s">
         <v>136</v>
@@ -52029,8 +52128,11 @@
       <c r="D187" s="14">
         <v>2</v>
       </c>
+      <c r="E187" s="40" t="s">
+        <v>231</v>
+      </c>
       <c r="F187" s="18" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="I187" s="29" t="s">
         <v>136</v>
@@ -52050,8 +52152,11 @@
       <c r="D188" s="14">
         <v>2</v>
       </c>
+      <c r="E188" s="40" t="s">
+        <v>232</v>
+      </c>
       <c r="F188" s="18" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="I188" s="29" t="s">
         <v>136</v>
@@ -52071,8 +52176,11 @@
       <c r="D189" s="14">
         <v>2</v>
       </c>
+      <c r="E189" s="40" t="s">
+        <v>233</v>
+      </c>
       <c r="F189" s="18" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="I189" s="29" t="s">
         <v>136</v>
@@ -52096,7 +52204,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -52113,7 +52221,7 @@
       <selection sqref="A1:XFD81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:37">
       <c r="A1">
@@ -61287,7 +61395,7 @@
       <selection sqref="A1:XFD81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:37">
       <c r="A1">
@@ -70461,7 +70569,7 @@
       <selection sqref="A1:XFD83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:37">
       <c r="A1">
@@ -79861,7 +79969,7 @@
       <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:37">
       <c r="A1">

</xml_diff>